<commit_message>
agregado borrado y adicion de archivos adjuntos a la accion de transicion
</commit_message>
<xml_diff>
--- a/public/uploads/6-a-Cotizacion-internet-plantilla.xlsx
+++ b/public/uploads/6-a-Cotizacion-internet-plantilla.xlsx
@@ -1672,17 +1672,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
     <numFmt numFmtId="170" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* \-??_ ;_-@_ "/>
     <numFmt numFmtId="171" formatCode="_ \$* #,##0.00_ ;_ \$* \-#,##0.00_ ;_ \$* \-??_ ;_ @_ "/>
     <numFmt numFmtId="172" formatCode="\$#,##0.00_);[RED]&quot;($&quot;#,##0.00\)"/>
-    <numFmt numFmtId="173" formatCode="0.00\ %"/>
+    <numFmt numFmtId="173" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
+    <numFmt numFmtId="174" formatCode="0.00\ %"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1796,14 +1797,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Century Gothic"/>
+      <sz val="9"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1908,7 +1909,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1955,13 +1956,6 @@
       <right style="medium"/>
       <top style="medium"/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -2230,79 +2224,75 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="12" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="18" fillId="3" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="14" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="13" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="16" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="15" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="20" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="20" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="20" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="11" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="10" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2314,7 +2304,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2326,11 +2316,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="173" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2459,9 +2453,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38880</xdr:colOff>
+      <xdr:colOff>38520</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2475,7 +2469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="361800" y="828360"/>
-          <a:ext cx="1839600" cy="693720"/>
+          <a:ext cx="1839240" cy="693360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2496,9 +2490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>28080</xdr:colOff>
+      <xdr:colOff>27720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2508,7 +2502,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="230760" y="3076920"/>
-          <a:ext cx="6897240" cy="1007280"/>
+          <a:ext cx="6896880" cy="1006920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2581,9 +2575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>28080</xdr:colOff>
+      <xdr:colOff>27720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2593,7 +2587,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="261000" y="1609560"/>
-          <a:ext cx="6867000" cy="1188360"/>
+          <a:ext cx="6866640" cy="1188000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2667,8 +2661,8 @@
   </sheetPr>
   <dimension ref="A1:N652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3043,32 +3037,32 @@
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="I24" s="39" t="e">
-        <f aca="false">H24*B24</f>
+      <c r="I24" s="38" t="e">
+        <f aca="false">B24*H24</f>
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="34"/>
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
-      <c r="B25" s="40" t="n">
+      <c r="B25" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42" t="s">
+      <c r="C25" s="40"/>
+      <c r="D25" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="43" t="str">
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42" t="str">
         <f aca="false">D36</f>
         <v>${NODO_NOD_COSTO_INSTALACION_CLIENTE}</v>
       </c>
-      <c r="I25" s="44" t="str">
+      <c r="I25" s="43" t="str">
         <f aca="false">D36</f>
         <v>${NODO_NOD_COSTO_INSTALACION_CLIENTE}</v>
       </c>
@@ -3076,17 +3070,17 @@
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="H26" s="46" t="s">
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="H26" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="47" t="e">
+      <c r="I26" s="46" t="e">
         <f aca="false">SUM(I24:I25)</f>
         <v>#VALUE!</v>
       </c>
@@ -3094,15 +3088,15 @@
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="H27" s="48" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="H27" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="49" t="e">
+      <c r="I27" s="48" t="e">
         <f aca="false">I26*14/100</f>
         <v>#VALUE!</v>
       </c>
@@ -3110,26 +3104,26 @@
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="51"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
       <c r="J28" s="34"/>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="H29" s="52" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="53" t="e">
+      <c r="I29" s="52" t="e">
         <f aca="false">I26+I27+I28</f>
         <v>#VALUE!</v>
       </c>
@@ -3141,33 +3135,33 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
       <c r="J30" s="34"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="57"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="34"/>
     </row>
     <row r="32" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
-      <c r="C32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
+      <c r="C32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
       <c r="I32" s="58"/>
       <c r="J32" s="34"/>
     </row>
@@ -3176,15 +3170,15 @@
       <c r="B33" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="58"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="60" t="n">
         <v>0.996</v>
       </c>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
       <c r="J33" s="34"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3192,15 +3186,15 @@
       <c r="B34" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="58"/>
+      <c r="C34" s="57"/>
       <c r="D34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
       <c r="J34" s="34"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3216,52 +3210,52 @@
       <c r="B36" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
       <c r="J36" s="34"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="57"/>
       <c r="D37" s="62" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="62"/>
       <c r="F37" s="62"/>
       <c r="G37" s="62"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
       <c r="J37" s="34"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="58"/>
+      <c r="C38" s="57"/>
       <c r="D38" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
       <c r="J38" s="34"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="57" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="63"/>

</xml_diff>

<commit_message>
ticket 83: ajustada la plantilla 6-a y 6-b de cotizaciones
</commit_message>
<xml_diff>
--- a/public/uploads/6-a-Cotizacion-internet-plantilla.xlsx
+++ b/public/uploads/6-a-Cotizacion-internet-plantilla.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="549">
   <si>
     <t xml:space="preserve">Empresa:</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t xml:space="preserve">${PRECIO_MB}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${PRECIO_CAPACIDAD}</t>
   </si>
   <si>
     <t xml:space="preserve">Instalación del Servicio</t>
@@ -162,10 +165,19 @@
     <t xml:space="preserve">SUBTOTAL A+B+C:</t>
   </si>
   <si>
+    <t xml:space="preserve">${SUBTOTAL_SERVICIO}</t>
+  </si>
+  <si>
     <t xml:space="preserve">12% IVA:</t>
   </si>
   <si>
+    <t xml:space="preserve">${IVA_SERVICIO}</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOTAL :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${TOTAL_SERVICIO}</t>
   </si>
   <si>
     <t xml:space="preserve">Condiciones comerciales</t>
@@ -2453,9 +2465,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38520</xdr:colOff>
+      <xdr:colOff>38160</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>102600</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2469,7 +2481,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="361800" y="828360"/>
-          <a:ext cx="1839240" cy="693360"/>
+          <a:ext cx="1838880" cy="693000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2490,9 +2502,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>27720</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>64440</xdr:rowOff>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2502,7 +2514,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="230760" y="3076920"/>
-          <a:ext cx="6896880" cy="1006920"/>
+          <a:ext cx="6896520" cy="1006560"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2575,9 +2587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>27720</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2587,7 +2599,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="261000" y="1609560"/>
-          <a:ext cx="6866640" cy="1188000"/>
+          <a:ext cx="6866280" cy="1187640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2661,8 +2673,8 @@
   </sheetPr>
   <dimension ref="A1:N652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3040,9 +3052,8 @@
       <c r="H24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="I24" s="38" t="e">
-        <f aca="false">B24*H24</f>
-        <v>#VALUE!</v>
+      <c r="I24" s="38" t="s">
+        <v>40</v>
       </c>
       <c r="J24" s="34"/>
     </row>
@@ -3053,7 +3064,7 @@
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
@@ -3071,18 +3082,17 @@
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" s="44"/>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
       <c r="F26" s="44"/>
       <c r="H26" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="46" t="e">
-        <f aca="false">SUM(I24:I25)</f>
-        <v>#VALUE!</v>
+        <v>43</v>
+      </c>
+      <c r="I26" s="46" t="s">
+        <v>44</v>
       </c>
       <c r="J26" s="34"/>
     </row>
@@ -3094,11 +3104,10 @@
       <c r="E27" s="44"/>
       <c r="F27" s="44"/>
       <c r="H27" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="I27" s="48" t="e">
-        <f aca="false">I26*14/100</f>
-        <v>#VALUE!</v>
+        <v>45</v>
+      </c>
+      <c r="I27" s="48" t="s">
+        <v>46</v>
       </c>
       <c r="J27" s="34"/>
     </row>
@@ -3121,11 +3130,10 @@
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
       <c r="H29" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="52" t="e">
-        <f aca="false">I26+I27+I28</f>
-        <v>#VALUE!</v>
+        <v>47</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>48</v>
       </c>
       <c r="J29" s="34"/>
     </row>
@@ -3144,7 +3152,7 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="55" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
@@ -3168,7 +3176,7 @@
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="59" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="60" t="n">
@@ -3184,11 +3192,11 @@
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="59" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E34" s="57"/>
       <c r="F34" s="57"/>
@@ -3199,20 +3207,20 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="59" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D35" s="61" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="59" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="61" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E36" s="57"/>
       <c r="F36" s="57"/>
@@ -3224,11 +3232,11 @@
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="57" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="62" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E37" s="62"/>
       <c r="F37" s="62"/>
@@ -3240,11 +3248,11 @@
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="57" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="63" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E38" s="57"/>
       <c r="F38" s="57"/>
@@ -3256,11 +3264,11 @@
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="57" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C39" s="63"/>
       <c r="D39" s="63" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E39" s="63"/>
       <c r="F39" s="63"/>
@@ -3298,12 +3306,12 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="64" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E42" s="65"/>
       <c r="F42" s="65"/>
       <c r="G42" s="66" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -3314,7 +3322,7 @@
       <c r="B43" s="67"/>
       <c r="C43" s="25"/>
       <c r="D43" s="68" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E43" s="25"/>
       <c r="F43" s="67"/>
@@ -3343,511 +3351,511 @@
     <row r="49" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D49" s="70"/>
       <c r="M49" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D50" s="70"/>
       <c r="M50" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D51" s="70"/>
       <c r="M51" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D52" s="70"/>
       <c r="M52" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D53" s="70"/>
       <c r="M53" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D54" s="70"/>
       <c r="M54" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D55" s="70"/>
       <c r="M55" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D56" s="70"/>
       <c r="M56" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D57" s="70"/>
       <c r="M57" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D58" s="70"/>
       <c r="M58" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D59" s="70"/>
       <c r="M59" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D60" s="70"/>
       <c r="E60" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D61" s="70"/>
       <c r="M61" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D62" s="70"/>
       <c r="M62" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D63" s="70"/>
       <c r="M63" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D64" s="70"/>
       <c r="M64" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D65" s="70"/>
       <c r="M65" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D66" s="70"/>
       <c r="M66" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D67" s="70"/>
       <c r="M67" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D68" s="70"/>
       <c r="M68" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D69" s="70"/>
       <c r="M69" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D70" s="70"/>
       <c r="M70" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D71" s="70"/>
       <c r="M71" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D72" s="70"/>
       <c r="M72" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D73" s="70"/>
       <c r="M73" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D74" s="70"/>
       <c r="M74" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="70"/>
       <c r="M75" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="70"/>
       <c r="M76" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="70"/>
       <c r="M77" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D78" s="70"/>
       <c r="M78" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="70"/>
       <c r="M79" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="70"/>
       <c r="M80" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="70"/>
       <c r="M81" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="70"/>
       <c r="M82" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="70"/>
       <c r="M83" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D84" s="70"/>
       <c r="M84" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D85" s="70"/>
       <c r="M85" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D86" s="70"/>
       <c r="M86" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D87" s="70"/>
       <c r="M87" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D88" s="70"/>
       <c r="M88" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D89" s="70"/>
       <c r="M89" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D90" s="70"/>
       <c r="M90" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D91" s="70"/>
       <c r="M91" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D92" s="70"/>
       <c r="M92" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D93" s="70"/>
       <c r="M93" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D94" s="70"/>
       <c r="M94" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D95" s="70"/>
       <c r="M95" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D96" s="70"/>
       <c r="M96" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D97" s="70"/>
       <c r="M97" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D98" s="70"/>
       <c r="M98" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D99" s="70"/>
       <c r="M99" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D100" s="70"/>
       <c r="M100" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D101" s="70"/>
       <c r="M101" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D102" s="70"/>
       <c r="M102" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D103" s="70"/>
       <c r="M103" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D104" s="70"/>
       <c r="M104" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3856,505 +3864,505 @@
     <row r="106" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D106" s="70"/>
       <c r="M106" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D107" s="70"/>
       <c r="M107" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D108" s="70"/>
       <c r="M108" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D109" s="70"/>
       <c r="M109" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D110" s="70"/>
       <c r="M110" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D111" s="70"/>
       <c r="M111" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D112" s="70"/>
       <c r="M112" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D113" s="70"/>
       <c r="M113" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D114" s="70"/>
       <c r="M114" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D115" s="70"/>
       <c r="M115" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D116" s="70"/>
       <c r="M116" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D117" s="70"/>
       <c r="M117" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D118" s="70"/>
       <c r="M118" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D119" s="70"/>
       <c r="M119" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D120" s="70"/>
       <c r="M120" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D121" s="70"/>
       <c r="M121" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D122" s="70"/>
       <c r="M122" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D123" s="70"/>
       <c r="M123" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D124" s="70"/>
       <c r="M124" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D125" s="70"/>
       <c r="M125" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D126" s="70"/>
       <c r="M126" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D127" s="70"/>
       <c r="M127" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D128" s="70"/>
       <c r="M128" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D129" s="70"/>
       <c r="M129" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D130" s="70"/>
       <c r="M130" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D131" s="70"/>
       <c r="M131" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D132" s="70"/>
       <c r="M132" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D133" s="70"/>
       <c r="M133" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D134" s="70"/>
       <c r="M134" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D135" s="70"/>
       <c r="M135" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D136" s="70"/>
       <c r="M136" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N136" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="N136" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D137" s="70"/>
       <c r="M137" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D138" s="70"/>
       <c r="M138" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D139" s="70"/>
       <c r="M139" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D140" s="70"/>
       <c r="M140" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D141" s="70"/>
       <c r="M141" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D142" s="70"/>
       <c r="M142" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D143" s="70"/>
       <c r="M143" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D144" s="70"/>
       <c r="M144" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D145" s="70"/>
       <c r="M145" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D146" s="70"/>
       <c r="M146" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D147" s="70"/>
       <c r="M147" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D148" s="70"/>
       <c r="M148" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D149" s="70"/>
       <c r="M149" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D150" s="70"/>
       <c r="M150" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D151" s="70"/>
       <c r="M151" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D152" s="70"/>
       <c r="M152" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D153" s="70"/>
       <c r="M153" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D154" s="70"/>
       <c r="M154" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D155" s="70"/>
       <c r="M155" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D156" s="70"/>
       <c r="M156" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D157" s="70"/>
       <c r="M157" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D158" s="70"/>
       <c r="M158" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D159" s="70"/>
       <c r="M159" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D160" s="70"/>
       <c r="M160" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D161" s="70"/>
       <c r="M161" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4363,505 +4371,505 @@
     <row r="163" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D163" s="70"/>
       <c r="M163" s="1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D164" s="70"/>
       <c r="M164" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D165" s="70"/>
       <c r="M165" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D166" s="70"/>
       <c r="M166" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D167" s="70"/>
       <c r="M167" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D168" s="70"/>
       <c r="M168" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="N168" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D169" s="70"/>
       <c r="M169" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="N169" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D170" s="70"/>
       <c r="M170" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="N170" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D171" s="70"/>
       <c r="M171" s="1" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="N171" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D172" s="70"/>
       <c r="M172" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="N172" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D173" s="70"/>
       <c r="M173" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="N173" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D174" s="70"/>
       <c r="M174" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="N174" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D175" s="70"/>
       <c r="M175" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="N175" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D176" s="70"/>
       <c r="M176" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N176" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D177" s="70"/>
       <c r="M177" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="N177" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D178" s="70"/>
       <c r="M178" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="N178" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D179" s="70"/>
       <c r="M179" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="N179" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D180" s="70"/>
       <c r="M180" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="N180" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D181" s="70"/>
       <c r="M181" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="N181" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D182" s="70"/>
       <c r="M182" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="N182" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D183" s="70"/>
       <c r="M183" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N183" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D184" s="70"/>
       <c r="M184" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="N184" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D185" s="70"/>
       <c r="M185" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="N185" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D186" s="70"/>
       <c r="M186" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="N186" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D187" s="70"/>
       <c r="M187" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="N187" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D188" s="70"/>
       <c r="M188" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N188" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D189" s="70"/>
       <c r="M189" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="N189" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D190" s="70"/>
       <c r="M190" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="N190" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D191" s="70"/>
       <c r="M191" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="N191" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D192" s="70"/>
       <c r="M192" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="N192" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D193" s="70"/>
       <c r="M193" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="N193" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D194" s="70"/>
       <c r="M194" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="N194" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D195" s="70"/>
       <c r="M195" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="N195" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D196" s="70"/>
       <c r="M196" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="N196" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D197" s="70"/>
       <c r="M197" s="1" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="N197" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D198" s="70"/>
       <c r="M198" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="N198" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D199" s="70"/>
       <c r="M199" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="N199" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D200" s="70"/>
       <c r="M200" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="N200" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D201" s="70"/>
       <c r="M201" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="N201" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D202" s="70"/>
       <c r="M202" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N202" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D203" s="70"/>
       <c r="M203" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="N203" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="N203" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D204" s="70"/>
       <c r="M204" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="N204" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D205" s="70"/>
       <c r="M205" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="N205" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D206" s="70"/>
       <c r="M206" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="N206" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D207" s="70"/>
       <c r="M207" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="N207" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D208" s="70"/>
       <c r="M208" s="1" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="N208" s="1" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D209" s="70"/>
       <c r="M209" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="N209" s="1" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D210" s="70"/>
       <c r="M210" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="N210" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D211" s="70"/>
       <c r="M211" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="N211" s="1" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D212" s="70"/>
       <c r="M212" s="1" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="N212" s="1" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D213" s="70"/>
       <c r="M213" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="N213" s="1" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D214" s="70"/>
       <c r="M214" s="1" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="N214" s="1" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D215" s="70"/>
       <c r="M215" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="N215" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D216" s="70"/>
       <c r="M216" s="1" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="N216" s="1" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D217" s="70"/>
       <c r="M217" s="1" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="N217" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D218" s="70"/>
       <c r="M218" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="N218" s="1" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4870,505 +4878,505 @@
     <row r="220" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D220" s="70"/>
       <c r="M220" s="1" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="N220" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D221" s="70"/>
       <c r="M221" s="1" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="N221" s="1" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D222" s="70"/>
       <c r="M222" s="1" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="N222" s="1" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D223" s="70"/>
       <c r="M223" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D224" s="70"/>
       <c r="M224" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D225" s="70"/>
       <c r="M225" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="N225" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D226" s="70"/>
       <c r="M226" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D227" s="70"/>
       <c r="M227" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D228" s="70"/>
       <c r="M228" s="1" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D229" s="70"/>
       <c r="M229" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="N229" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D230" s="70"/>
       <c r="M230" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="N230" s="1" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D231" s="70"/>
       <c r="M231" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D232" s="70"/>
       <c r="M232" s="1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D233" s="70"/>
       <c r="M233" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="N233" s="1" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D234" s="70"/>
       <c r="M234" s="1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="N234" s="1" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D235" s="70"/>
       <c r="M235" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="N235" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D236" s="70"/>
       <c r="M236" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="N236" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D237" s="70"/>
       <c r="M237" s="1" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="N237" s="1" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D238" s="70"/>
       <c r="M238" s="1" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="N238" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D239" s="70"/>
       <c r="M239" s="1" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D240" s="70"/>
       <c r="M240" s="1" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D241" s="70"/>
       <c r="M241" s="1" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D242" s="70"/>
       <c r="M242" s="1" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D243" s="70"/>
       <c r="M243" s="1" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D244" s="70"/>
       <c r="M244" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D245" s="70"/>
       <c r="M245" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="N245" s="1" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D246" s="70"/>
       <c r="M246" s="1" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="N246" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D247" s="70"/>
       <c r="M247" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D248" s="70"/>
       <c r="M248" s="1" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D249" s="70"/>
       <c r="M249" s="1" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D250" s="70"/>
       <c r="M250" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D251" s="70"/>
       <c r="M251" s="1" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D252" s="70"/>
       <c r="M252" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D253" s="70"/>
       <c r="M253" s="1" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D254" s="70"/>
       <c r="M254" s="1" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D255" s="70"/>
       <c r="M255" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D256" s="70"/>
       <c r="M256" s="1" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D257" s="70"/>
       <c r="M257" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D258" s="70"/>
       <c r="M258" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D259" s="70"/>
       <c r="M259" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D260" s="70"/>
       <c r="M260" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D261" s="70"/>
       <c r="M261" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="N261" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D262" s="70"/>
       <c r="M262" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="N262" s="1" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D263" s="70"/>
       <c r="M263" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="N263" s="1" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D264" s="70"/>
       <c r="M264" s="1" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="N264" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D265" s="70"/>
       <c r="M265" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="N265" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D266" s="70"/>
       <c r="M266" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="N266" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D267" s="70"/>
       <c r="M267" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="N267" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D268" s="70"/>
       <c r="M268" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="N268" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D269" s="70"/>
       <c r="M269" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="N269" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D270" s="70"/>
       <c r="M270" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="N270" s="1" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D271" s="70"/>
       <c r="M271" s="1" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="N271" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D272" s="70"/>
       <c r="M272" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="N272" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D273" s="70"/>
       <c r="M273" s="1" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="N273" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D274" s="70"/>
       <c r="M274" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="N274" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D275" s="70"/>
       <c r="M275" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="N275" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5377,379 +5385,379 @@
     <row r="277" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D277" s="70"/>
       <c r="M277" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="N277" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D278" s="70"/>
       <c r="M278" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="N278" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D279" s="70"/>
       <c r="M279" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="N279" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D280" s="70"/>
       <c r="M280" s="1" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="N280" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D281" s="70"/>
       <c r="M281" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="N281" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D282" s="70"/>
       <c r="M282" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="N282" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D283" s="70"/>
       <c r="M283" s="1" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="N283" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D284" s="70"/>
       <c r="M284" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="N284" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D285" s="70"/>
       <c r="M285" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="N285" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D286" s="70"/>
       <c r="M286" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="N286" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D287" s="70"/>
       <c r="M287" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="N287" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D288" s="70"/>
       <c r="M288" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="N288" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D289" s="70"/>
       <c r="M289" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="N289" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D290" s="70"/>
       <c r="M290" s="1" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="N290" s="1" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D291" s="70"/>
       <c r="M291" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="N291" s="1" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D292" s="70"/>
       <c r="M292" s="1" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="N292" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D293" s="70"/>
       <c r="M293" s="1" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="N293" s="1" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D294" s="70"/>
       <c r="M294" s="1" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="N294" s="1" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D295" s="70"/>
       <c r="M295" s="1" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="N295" s="1" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D296" s="70"/>
       <c r="M296" s="1" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="N296" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D297" s="70"/>
       <c r="M297" s="1" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="N297" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D298" s="70"/>
       <c r="M298" s="1" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="N298" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D299" s="70"/>
       <c r="M299" s="1" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="N299" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D300" s="70"/>
       <c r="M300" s="1" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="N300" s="1" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D301" s="70"/>
       <c r="M301" s="1" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="N301" s="1" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D302" s="70"/>
       <c r="M302" s="1" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="N302" s="1" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D303" s="70"/>
       <c r="M303" s="1" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="N303" s="1" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D304" s="70"/>
       <c r="M304" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="N304" s="1" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D305" s="70"/>
       <c r="M305" s="1" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="N305" s="1" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D306" s="70"/>
       <c r="M306" s="1" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="N306" s="1" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D307" s="70"/>
       <c r="M307" s="1" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="N307" s="1" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D308" s="70"/>
       <c r="M308" s="1" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="N308" s="1" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D309" s="70"/>
       <c r="M309" s="1" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="N309" s="1" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D310" s="70"/>
       <c r="M310" s="1" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="N310" s="1" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D311" s="70"/>
       <c r="M311" s="1" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="N311" s="1" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D312" s="70"/>
       <c r="M312" s="1" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="N312" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D313" s="70"/>
       <c r="M313" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="N313" s="1" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D314" s="70"/>
       <c r="M314" s="1" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="N314" s="1" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D315" s="70"/>
       <c r="M315" s="1" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="N315" s="1" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D316" s="70"/>
       <c r="M316" s="1" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="N316" s="1" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D317" s="70"/>
       <c r="M317" s="1" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="N317" s="1" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D318" s="70"/>
       <c r="M318" s="1" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="N318" s="1" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>